<commit_message>
incluindo exportacoes do top 10
</commit_message>
<xml_diff>
--- a/top10.xlsx
+++ b/top10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandre/Library/Mobile Documents/com~apple~CloudDocs/PosTechFiap/FIAP/FASE 1 - DATA ANALYSIS AND EXPLORATION/4 - Tech Challenge/Exportacao/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E83D03-92E6-1C41-8445-742D06CA6F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E651DC69-429D-F04F-957B-01649C9F9CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21800" windowHeight="12980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="18">
   <si>
     <t>China</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Variavel</t>
+  </si>
+  <si>
+    <t>Exportação</t>
   </si>
 </sst>
 </file>
@@ -451,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47F90730-DE6E-4990-B5C3-FD64641F0A26}">
-  <dimension ref="A1:D429"/>
+  <dimension ref="A1:D564"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A456" workbookViewId="0">
+      <selection activeCell="A430" sqref="A430:D564"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6470,6 +6473,1896 @@
         <v>75600000</v>
       </c>
     </row>
+    <row r="430" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A430">
+        <v>2008</v>
+      </c>
+      <c r="B430" t="s">
+        <v>0</v>
+      </c>
+      <c r="C430" t="s">
+        <v>17</v>
+      </c>
+      <c r="D430" s="2">
+        <v>5400000</v>
+      </c>
+    </row>
+    <row r="431" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A431">
+        <v>2009</v>
+      </c>
+      <c r="B431" t="s">
+        <v>0</v>
+      </c>
+      <c r="C431" t="s">
+        <v>17</v>
+      </c>
+      <c r="D431" s="2">
+        <v>1500000</v>
+      </c>
+    </row>
+    <row r="432" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A432">
+        <v>2010</v>
+      </c>
+      <c r="B432" t="s">
+        <v>0</v>
+      </c>
+      <c r="C432" t="s">
+        <v>17</v>
+      </c>
+      <c r="D432" s="2">
+        <v>1500000</v>
+      </c>
+    </row>
+    <row r="433" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A433">
+        <v>2011</v>
+      </c>
+      <c r="B433" t="s">
+        <v>0</v>
+      </c>
+      <c r="C433" t="s">
+        <v>17</v>
+      </c>
+      <c r="D433" s="2">
+        <v>1900000</v>
+      </c>
+    </row>
+    <row r="434" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A434">
+        <v>2012</v>
+      </c>
+      <c r="B434" t="s">
+        <v>0</v>
+      </c>
+      <c r="C434" t="s">
+        <v>17</v>
+      </c>
+      <c r="D434" s="2">
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="435" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A435">
+        <v>2013</v>
+      </c>
+      <c r="B435" t="s">
+        <v>0</v>
+      </c>
+      <c r="C435" t="s">
+        <v>17</v>
+      </c>
+      <c r="D435" s="2">
+        <v>1900000</v>
+      </c>
+    </row>
+    <row r="436" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A436">
+        <v>2014</v>
+      </c>
+      <c r="B436" t="s">
+        <v>0</v>
+      </c>
+      <c r="C436" t="s">
+        <v>17</v>
+      </c>
+      <c r="D436" s="2">
+        <v>3700000</v>
+      </c>
+    </row>
+    <row r="437" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A437">
+        <v>2015</v>
+      </c>
+      <c r="B437" t="s">
+        <v>0</v>
+      </c>
+      <c r="C437" t="s">
+        <v>17</v>
+      </c>
+      <c r="D437" s="2">
+        <v>8200000</v>
+      </c>
+    </row>
+    <row r="438" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A438">
+        <v>2016</v>
+      </c>
+      <c r="B438" t="s">
+        <v>0</v>
+      </c>
+      <c r="C438" t="s">
+        <v>17</v>
+      </c>
+      <c r="D438" s="2">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="439" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A439">
+        <v>2017</v>
+      </c>
+      <c r="B439" t="s">
+        <v>0</v>
+      </c>
+      <c r="C439" t="s">
+        <v>17</v>
+      </c>
+      <c r="D439" s="2">
+        <v>9400000</v>
+      </c>
+    </row>
+    <row r="440" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A440">
+        <v>2018</v>
+      </c>
+      <c r="B440" t="s">
+        <v>0</v>
+      </c>
+      <c r="C440" t="s">
+        <v>17</v>
+      </c>
+      <c r="D440" s="2">
+        <v>6300000</v>
+      </c>
+    </row>
+    <row r="441" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A441">
+        <v>2019</v>
+      </c>
+      <c r="B441" t="s">
+        <v>0</v>
+      </c>
+      <c r="C441" t="s">
+        <v>17</v>
+      </c>
+      <c r="D441" s="2">
+        <v>3600000</v>
+      </c>
+    </row>
+    <row r="442" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A442">
+        <v>2020</v>
+      </c>
+      <c r="B442" t="s">
+        <v>0</v>
+      </c>
+      <c r="C442" t="s">
+        <v>17</v>
+      </c>
+      <c r="D442" s="2">
+        <v>1600000</v>
+      </c>
+    </row>
+    <row r="443" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A443">
+        <v>2021</v>
+      </c>
+      <c r="B443" t="s">
+        <v>0</v>
+      </c>
+      <c r="C443" t="s">
+        <v>17</v>
+      </c>
+      <c r="D443" s="2">
+        <v>4200000</v>
+      </c>
+    </row>
+    <row r="444" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A444">
+        <v>2022</v>
+      </c>
+      <c r="B444" t="s">
+        <v>0</v>
+      </c>
+      <c r="C444" t="s">
+        <v>17</v>
+      </c>
+      <c r="D444" s="2">
+        <v>2900000</v>
+      </c>
+    </row>
+    <row r="445" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A445">
+        <v>2008</v>
+      </c>
+      <c r="B445" t="s">
+        <v>5</v>
+      </c>
+      <c r="C445" t="s">
+        <v>17</v>
+      </c>
+      <c r="D445" s="2">
+        <v>358000000</v>
+      </c>
+    </row>
+    <row r="446" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A446">
+        <v>2009</v>
+      </c>
+      <c r="B446" t="s">
+        <v>5</v>
+      </c>
+      <c r="C446" t="s">
+        <v>17</v>
+      </c>
+      <c r="D446" s="2">
+        <v>355700000</v>
+      </c>
+    </row>
+    <row r="447" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A447">
+        <v>2010</v>
+      </c>
+      <c r="B447" t="s">
+        <v>5</v>
+      </c>
+      <c r="C447" t="s">
+        <v>17</v>
+      </c>
+      <c r="D447" s="2">
+        <v>392900000</v>
+      </c>
+    </row>
+    <row r="448" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A448">
+        <v>2011</v>
+      </c>
+      <c r="B448" t="s">
+        <v>5</v>
+      </c>
+      <c r="C448" t="s">
+        <v>17</v>
+      </c>
+      <c r="D448" s="2">
+        <v>414500000</v>
+      </c>
+    </row>
+    <row r="449" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A449">
+        <v>2012</v>
+      </c>
+      <c r="B449" t="s">
+        <v>5</v>
+      </c>
+      <c r="C449" t="s">
+        <v>17</v>
+      </c>
+      <c r="D449" s="2">
+        <v>397300000</v>
+      </c>
+    </row>
+    <row r="450" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A450">
+        <v>2013</v>
+      </c>
+      <c r="B450" t="s">
+        <v>5</v>
+      </c>
+      <c r="C450" t="s">
+        <v>17</v>
+      </c>
+      <c r="D450" s="2">
+        <v>390300000</v>
+      </c>
+    </row>
+    <row r="451" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A451">
+        <v>2014</v>
+      </c>
+      <c r="B451" t="s">
+        <v>5</v>
+      </c>
+      <c r="C451" t="s">
+        <v>17</v>
+      </c>
+      <c r="D451" s="2">
+        <v>367500000</v>
+      </c>
+    </row>
+    <row r="452" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A452">
+        <v>2015</v>
+      </c>
+      <c r="B452" t="s">
+        <v>5</v>
+      </c>
+      <c r="C452" t="s">
+        <v>17</v>
+      </c>
+      <c r="D452" s="2">
+        <v>392800000</v>
+      </c>
+    </row>
+    <row r="453" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A453">
+        <v>2016</v>
+      </c>
+      <c r="B453" t="s">
+        <v>5</v>
+      </c>
+      <c r="C453" t="s">
+        <v>17</v>
+      </c>
+      <c r="D453" s="2">
+        <v>360900000</v>
+      </c>
+    </row>
+    <row r="454" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A454">
+        <v>2017</v>
+      </c>
+      <c r="B454" t="s">
+        <v>5</v>
+      </c>
+      <c r="C454" t="s">
+        <v>17</v>
+      </c>
+      <c r="D454" s="2">
+        <v>383600000</v>
+      </c>
+    </row>
+    <row r="455" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A455">
+        <v>2018</v>
+      </c>
+      <c r="B455" t="s">
+        <v>5</v>
+      </c>
+      <c r="C455" t="s">
+        <v>17</v>
+      </c>
+      <c r="D455" s="2">
+        <v>373100000</v>
+      </c>
+    </row>
+    <row r="456" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A456">
+        <v>2019</v>
+      </c>
+      <c r="B456" t="s">
+        <v>5</v>
+      </c>
+      <c r="C456" t="s">
+        <v>17</v>
+      </c>
+      <c r="D456" s="2">
+        <v>383900000</v>
+      </c>
+    </row>
+    <row r="457" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A457">
+        <v>2020</v>
+      </c>
+      <c r="B457" t="s">
+        <v>5</v>
+      </c>
+      <c r="C457" t="s">
+        <v>17</v>
+      </c>
+      <c r="D457" s="2">
+        <v>366200000</v>
+      </c>
+    </row>
+    <row r="458" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A458">
+        <v>2021</v>
+      </c>
+      <c r="B458" t="s">
+        <v>5</v>
+      </c>
+      <c r="C458" t="s">
+        <v>17</v>
+      </c>
+      <c r="D458" s="2">
+        <v>368900000</v>
+      </c>
+    </row>
+    <row r="459" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A459">
+        <v>2022</v>
+      </c>
+      <c r="B459" t="s">
+        <v>5</v>
+      </c>
+      <c r="C459" t="s">
+        <v>17</v>
+      </c>
+      <c r="D459" s="2">
+        <v>353300000</v>
+      </c>
+    </row>
+    <row r="460" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A460">
+        <v>2008</v>
+      </c>
+      <c r="B460" t="s">
+        <v>6</v>
+      </c>
+      <c r="C460" t="s">
+        <v>17</v>
+      </c>
+      <c r="D460" s="2">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="461" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A461">
+        <v>2009</v>
+      </c>
+      <c r="B461" t="s">
+        <v>6</v>
+      </c>
+      <c r="C461" t="s">
+        <v>17</v>
+      </c>
+      <c r="D461" s="2">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="462" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A462">
+        <v>2010</v>
+      </c>
+      <c r="B462" t="s">
+        <v>6</v>
+      </c>
+      <c r="C462" t="s">
+        <v>17</v>
+      </c>
+      <c r="D462" s="2">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="463" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A463">
+        <v>2011</v>
+      </c>
+      <c r="B463" t="s">
+        <v>6</v>
+      </c>
+      <c r="C463" t="s">
+        <v>17</v>
+      </c>
+      <c r="D463" s="2">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="464" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A464">
+        <v>2012</v>
+      </c>
+      <c r="B464" t="s">
+        <v>6</v>
+      </c>
+      <c r="C464" t="s">
+        <v>17</v>
+      </c>
+      <c r="D464" s="2">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="465" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A465">
+        <v>2013</v>
+      </c>
+      <c r="B465" t="s">
+        <v>6</v>
+      </c>
+      <c r="C465" t="s">
+        <v>17</v>
+      </c>
+      <c r="D465" s="2">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="466" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A466">
+        <v>2014</v>
+      </c>
+      <c r="B466" t="s">
+        <v>6</v>
+      </c>
+      <c r="C466" t="s">
+        <v>17</v>
+      </c>
+      <c r="D466" s="2">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="467" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A467">
+        <v>2015</v>
+      </c>
+      <c r="B467" t="s">
+        <v>6</v>
+      </c>
+      <c r="C467" t="s">
+        <v>17</v>
+      </c>
+      <c r="D467" s="2">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="468" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A468">
+        <v>2016</v>
+      </c>
+      <c r="B468" t="s">
+        <v>6</v>
+      </c>
+      <c r="C468" t="s">
+        <v>17</v>
+      </c>
+      <c r="D468" s="2">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="469" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A469">
+        <v>2017</v>
+      </c>
+      <c r="B469" t="s">
+        <v>6</v>
+      </c>
+      <c r="C469" t="s">
+        <v>17</v>
+      </c>
+      <c r="D469" s="2">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="470" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A470">
+        <v>2018</v>
+      </c>
+      <c r="B470" t="s">
+        <v>6</v>
+      </c>
+      <c r="C470" t="s">
+        <v>17</v>
+      </c>
+      <c r="D470" s="2">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="471" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A471">
+        <v>2019</v>
+      </c>
+      <c r="B471" t="s">
+        <v>6</v>
+      </c>
+      <c r="C471" t="s">
+        <v>17</v>
+      </c>
+      <c r="D471" s="2">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="472" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A472">
+        <v>2020</v>
+      </c>
+      <c r="B472" t="s">
+        <v>6</v>
+      </c>
+      <c r="C472" t="s">
+        <v>17</v>
+      </c>
+      <c r="D472" s="2">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="473" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A473">
+        <v>2021</v>
+      </c>
+      <c r="B473" t="s">
+        <v>6</v>
+      </c>
+      <c r="C473" t="s">
+        <v>17</v>
+      </c>
+      <c r="D473" s="2">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="474" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A474">
+        <v>2022</v>
+      </c>
+      <c r="B474" t="s">
+        <v>6</v>
+      </c>
+      <c r="C474" t="s">
+        <v>17</v>
+      </c>
+      <c r="D474" s="2">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="475" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A475">
+        <v>2008</v>
+      </c>
+      <c r="B475" t="s">
+        <v>7</v>
+      </c>
+      <c r="C475" t="s">
+        <v>17</v>
+      </c>
+      <c r="D475" s="2">
+        <v>17700000</v>
+      </c>
+    </row>
+    <row r="476" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A476">
+        <v>2009</v>
+      </c>
+      <c r="B476" t="s">
+        <v>7</v>
+      </c>
+      <c r="C476" t="s">
+        <v>17</v>
+      </c>
+      <c r="D476" s="2">
+        <v>16700000</v>
+      </c>
+    </row>
+    <row r="477" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A477">
+        <v>2010</v>
+      </c>
+      <c r="B477" t="s">
+        <v>7</v>
+      </c>
+      <c r="C477" t="s">
+        <v>17</v>
+      </c>
+      <c r="D477" s="2">
+        <v>14900000</v>
+      </c>
+    </row>
+    <row r="478" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A478">
+        <v>2011</v>
+      </c>
+      <c r="B478" t="s">
+        <v>7</v>
+      </c>
+      <c r="C478" t="s">
+        <v>17</v>
+      </c>
+      <c r="D478" s="2">
+        <v>24400000</v>
+      </c>
+    </row>
+    <row r="479" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A479">
+        <v>2012</v>
+      </c>
+      <c r="B479" t="s">
+        <v>7</v>
+      </c>
+      <c r="C479" t="s">
+        <v>17</v>
+      </c>
+      <c r="D479" s="2">
+        <v>28200000</v>
+      </c>
+    </row>
+    <row r="480" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A480">
+        <v>2013</v>
+      </c>
+      <c r="B480" t="s">
+        <v>7</v>
+      </c>
+      <c r="C480" t="s">
+        <v>17</v>
+      </c>
+      <c r="D480" s="2">
+        <v>25800000</v>
+      </c>
+    </row>
+    <row r="481" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A481">
+        <v>2014</v>
+      </c>
+      <c r="B481" t="s">
+        <v>7</v>
+      </c>
+      <c r="C481" t="s">
+        <v>17</v>
+      </c>
+      <c r="D481" s="2">
+        <v>31300000</v>
+      </c>
+    </row>
+    <row r="482" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A482">
+        <v>2015</v>
+      </c>
+      <c r="B482" t="s">
+        <v>7</v>
+      </c>
+      <c r="C482" t="s">
+        <v>17</v>
+      </c>
+      <c r="D482" s="2">
+        <v>37600000</v>
+      </c>
+    </row>
+    <row r="483" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A483">
+        <v>2016</v>
+      </c>
+      <c r="B483" t="s">
+        <v>7</v>
+      </c>
+      <c r="C483" t="s">
+        <v>17</v>
+      </c>
+      <c r="D483" s="2">
+        <v>66800000</v>
+      </c>
+    </row>
+    <row r="484" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A484">
+        <v>2017</v>
+      </c>
+      <c r="B484" t="s">
+        <v>7</v>
+      </c>
+      <c r="C484" t="s">
+        <v>17</v>
+      </c>
+      <c r="D484" s="2">
+        <v>79500000</v>
+      </c>
+    </row>
+    <row r="485" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A485">
+        <v>2018</v>
+      </c>
+      <c r="B485" t="s">
+        <v>7</v>
+      </c>
+      <c r="C485" t="s">
+        <v>17</v>
+      </c>
+      <c r="D485" s="2">
+        <v>72700000</v>
+      </c>
+    </row>
+    <row r="486" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A486">
+        <v>2019</v>
+      </c>
+      <c r="B486" t="s">
+        <v>7</v>
+      </c>
+      <c r="C486" t="s">
+        <v>17</v>
+      </c>
+      <c r="D486" s="2">
+        <v>64900000</v>
+      </c>
+    </row>
+    <row r="487" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A487">
+        <v>2020</v>
+      </c>
+      <c r="B487" t="s">
+        <v>7</v>
+      </c>
+      <c r="C487" t="s">
+        <v>17</v>
+      </c>
+      <c r="D487" s="2">
+        <v>96000000</v>
+      </c>
+    </row>
+    <row r="488" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A488">
+        <v>2021</v>
+      </c>
+      <c r="B488" t="s">
+        <v>7</v>
+      </c>
+      <c r="C488" t="s">
+        <v>17</v>
+      </c>
+      <c r="D488" s="2">
+        <v>116500000</v>
+      </c>
+    </row>
+    <row r="489" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A489">
+        <v>2022</v>
+      </c>
+      <c r="B489" t="s">
+        <v>7</v>
+      </c>
+      <c r="C489" t="s">
+        <v>17</v>
+      </c>
+      <c r="D489" s="2">
+        <v>112300000</v>
+      </c>
+    </row>
+    <row r="490" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A490">
+        <v>2008</v>
+      </c>
+      <c r="B490" t="s">
+        <v>9</v>
+      </c>
+      <c r="C490" t="s">
+        <v>17</v>
+      </c>
+      <c r="D490" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="491" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A491">
+        <v>2009</v>
+      </c>
+      <c r="B491" t="s">
+        <v>9</v>
+      </c>
+      <c r="C491" t="s">
+        <v>17</v>
+      </c>
+      <c r="D491" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="492" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A492">
+        <v>2010</v>
+      </c>
+      <c r="B492" t="s">
+        <v>9</v>
+      </c>
+      <c r="C492" t="s">
+        <v>17</v>
+      </c>
+      <c r="D492" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="493" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A493">
+        <v>2011</v>
+      </c>
+      <c r="B493" t="s">
+        <v>9</v>
+      </c>
+      <c r="C493" t="s">
+        <v>17</v>
+      </c>
+      <c r="D493" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="494" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A494">
+        <v>2012</v>
+      </c>
+      <c r="B494" t="s">
+        <v>9</v>
+      </c>
+      <c r="C494" t="s">
+        <v>17</v>
+      </c>
+      <c r="D494" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="495" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A495">
+        <v>2013</v>
+      </c>
+      <c r="B495" t="s">
+        <v>9</v>
+      </c>
+      <c r="C495" t="s">
+        <v>17</v>
+      </c>
+      <c r="D495" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="496" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A496">
+        <v>2014</v>
+      </c>
+      <c r="B496" t="s">
+        <v>9</v>
+      </c>
+      <c r="C496" t="s">
+        <v>17</v>
+      </c>
+      <c r="D496" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="497" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A497">
+        <v>2015</v>
+      </c>
+      <c r="B497" t="s">
+        <v>9</v>
+      </c>
+      <c r="C497" t="s">
+        <v>17</v>
+      </c>
+      <c r="D497" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="498" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A498">
+        <v>2016</v>
+      </c>
+      <c r="B498" t="s">
+        <v>9</v>
+      </c>
+      <c r="C498" t="s">
+        <v>17</v>
+      </c>
+      <c r="D498" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="499" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A499">
+        <v>2017</v>
+      </c>
+      <c r="B499" t="s">
+        <v>9</v>
+      </c>
+      <c r="C499" t="s">
+        <v>17</v>
+      </c>
+      <c r="D499" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="500" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A500">
+        <v>2018</v>
+      </c>
+      <c r="B500" t="s">
+        <v>9</v>
+      </c>
+      <c r="C500" t="s">
+        <v>17</v>
+      </c>
+      <c r="D500" s="2">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="501" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A501">
+        <v>2019</v>
+      </c>
+      <c r="B501" t="s">
+        <v>9</v>
+      </c>
+      <c r="C501" t="s">
+        <v>17</v>
+      </c>
+      <c r="D501" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="502" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A502">
+        <v>2020</v>
+      </c>
+      <c r="B502" t="s">
+        <v>9</v>
+      </c>
+      <c r="C502" t="s">
+        <v>17</v>
+      </c>
+      <c r="D502" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="503" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A503">
+        <v>2021</v>
+      </c>
+      <c r="B503" t="s">
+        <v>9</v>
+      </c>
+      <c r="C503" t="s">
+        <v>17</v>
+      </c>
+      <c r="D503" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="504" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A504">
+        <v>2022</v>
+      </c>
+      <c r="B504" t="s">
+        <v>9</v>
+      </c>
+      <c r="C504" t="s">
+        <v>17</v>
+      </c>
+      <c r="D504" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="505" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A505">
+        <v>2008</v>
+      </c>
+      <c r="B505" t="s">
+        <v>8</v>
+      </c>
+      <c r="C505" t="s">
+        <v>17</v>
+      </c>
+      <c r="D505" s="2">
+        <v>1691400000</v>
+      </c>
+    </row>
+    <row r="506" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A506">
+        <v>2009</v>
+      </c>
+      <c r="B506" t="s">
+        <v>8</v>
+      </c>
+      <c r="C506" t="s">
+        <v>17</v>
+      </c>
+      <c r="D506" s="2">
+        <v>1460700000</v>
+      </c>
+    </row>
+    <row r="507" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A507">
+        <v>2010</v>
+      </c>
+      <c r="B507" t="s">
+        <v>8</v>
+      </c>
+      <c r="C507" t="s">
+        <v>17</v>
+      </c>
+      <c r="D507" s="2">
+        <v>1715600000</v>
+      </c>
+    </row>
+    <row r="508" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A508">
+        <v>2011</v>
+      </c>
+      <c r="B508" t="s">
+        <v>8</v>
+      </c>
+      <c r="C508" t="s">
+        <v>17</v>
+      </c>
+      <c r="D508" s="2">
+        <v>2203100000</v>
+      </c>
+    </row>
+    <row r="509" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A509">
+        <v>2012</v>
+      </c>
+      <c r="B509" t="s">
+        <v>8</v>
+      </c>
+      <c r="C509" t="s">
+        <v>17</v>
+      </c>
+      <c r="D509" s="2">
+        <v>2141100000</v>
+      </c>
+    </row>
+    <row r="510" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A510">
+        <v>2013</v>
+      </c>
+      <c r="B510" t="s">
+        <v>8</v>
+      </c>
+      <c r="C510" t="s">
+        <v>17</v>
+      </c>
+      <c r="D510" s="2">
+        <v>1845000000</v>
+      </c>
+    </row>
+    <row r="511" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A511">
+        <v>2014</v>
+      </c>
+      <c r="B511" t="s">
+        <v>8</v>
+      </c>
+      <c r="C511" t="s">
+        <v>17</v>
+      </c>
+      <c r="D511" s="2">
+        <v>2308800000</v>
+      </c>
+    </row>
+    <row r="512" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A512">
+        <v>2015</v>
+      </c>
+      <c r="B512" t="s">
+        <v>8</v>
+      </c>
+      <c r="C512" t="s">
+        <v>17</v>
+      </c>
+      <c r="D512" s="2">
+        <v>2439500000</v>
+      </c>
+    </row>
+    <row r="513" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A513">
+        <v>2016</v>
+      </c>
+      <c r="B513" t="s">
+        <v>8</v>
+      </c>
+      <c r="C513" t="s">
+        <v>17</v>
+      </c>
+      <c r="D513" s="2">
+        <v>2262600000</v>
+      </c>
+    </row>
+    <row r="514" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A514">
+        <v>2017</v>
+      </c>
+      <c r="B514" t="s">
+        <v>8</v>
+      </c>
+      <c r="C514" t="s">
+        <v>17</v>
+      </c>
+      <c r="D514" s="2">
+        <v>2331100000</v>
+      </c>
+    </row>
+    <row r="515" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A515">
+        <v>2018</v>
+      </c>
+      <c r="B515" t="s">
+        <v>8</v>
+      </c>
+      <c r="C515" t="s">
+        <v>17</v>
+      </c>
+      <c r="D515" s="2">
+        <v>2030800000</v>
+      </c>
+    </row>
+    <row r="516" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A516">
+        <v>2019</v>
+      </c>
+      <c r="B516" t="s">
+        <v>8</v>
+      </c>
+      <c r="C516" t="s">
+        <v>17</v>
+      </c>
+      <c r="D516" s="2">
+        <v>2138700000</v>
+      </c>
+    </row>
+    <row r="517" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A517">
+        <v>2020</v>
+      </c>
+      <c r="B517" t="s">
+        <v>8</v>
+      </c>
+      <c r="C517" t="s">
+        <v>17</v>
+      </c>
+      <c r="D517" s="2">
+        <v>2017200000</v>
+      </c>
+    </row>
+    <row r="518" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A518">
+        <v>2021</v>
+      </c>
+      <c r="B518" t="s">
+        <v>8</v>
+      </c>
+      <c r="C518" t="s">
+        <v>17</v>
+      </c>
+      <c r="D518" s="2">
+        <v>2298500000</v>
+      </c>
+    </row>
+    <row r="519" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A519">
+        <v>2022</v>
+      </c>
+      <c r="B519" t="s">
+        <v>8</v>
+      </c>
+      <c r="C519" t="s">
+        <v>17</v>
+      </c>
+      <c r="D519" s="2">
+        <v>2089500000</v>
+      </c>
+    </row>
+    <row r="520" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A520">
+        <v>2008</v>
+      </c>
+      <c r="B520" t="s">
+        <v>11</v>
+      </c>
+      <c r="C520" t="s">
+        <v>17</v>
+      </c>
+      <c r="D520" s="2">
+        <v>43300000</v>
+      </c>
+    </row>
+    <row r="521" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A521">
+        <v>2009</v>
+      </c>
+      <c r="B521" t="s">
+        <v>11</v>
+      </c>
+      <c r="C521" t="s">
+        <v>17</v>
+      </c>
+      <c r="D521" s="2">
+        <v>54500000</v>
+      </c>
+    </row>
+    <row r="522" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A522">
+        <v>2010</v>
+      </c>
+      <c r="B522" t="s">
+        <v>11</v>
+      </c>
+      <c r="C522" t="s">
+        <v>17</v>
+      </c>
+      <c r="D522" s="2">
+        <v>89800000</v>
+      </c>
+    </row>
+    <row r="523" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A523">
+        <v>2011</v>
+      </c>
+      <c r="B523" t="s">
+        <v>11</v>
+      </c>
+      <c r="C523" t="s">
+        <v>17</v>
+      </c>
+      <c r="D523" s="2">
+        <v>86600000</v>
+      </c>
+    </row>
+    <row r="524" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A524">
+        <v>2012</v>
+      </c>
+      <c r="B524" t="s">
+        <v>11</v>
+      </c>
+      <c r="C524" t="s">
+        <v>17</v>
+      </c>
+      <c r="D524" s="2">
+        <v>80000000</v>
+      </c>
+    </row>
+    <row r="525" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A525">
+        <v>2013</v>
+      </c>
+      <c r="B525" t="s">
+        <v>11</v>
+      </c>
+      <c r="C525" t="s">
+        <v>17</v>
+      </c>
+      <c r="D525" s="2">
+        <v>95100000</v>
+      </c>
+    </row>
+    <row r="526" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A526">
+        <v>2014</v>
+      </c>
+      <c r="B526" t="s">
+        <v>11</v>
+      </c>
+      <c r="C526" t="s">
+        <v>17</v>
+      </c>
+      <c r="D526" s="2">
+        <v>103700000</v>
+      </c>
+    </row>
+    <row r="527" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A527">
+        <v>2015</v>
+      </c>
+      <c r="B527" t="s">
+        <v>11</v>
+      </c>
+      <c r="C527" t="s">
+        <v>17</v>
+      </c>
+      <c r="D527" s="2">
+        <v>94200000</v>
+      </c>
+    </row>
+    <row r="528" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A528">
+        <v>2016</v>
+      </c>
+      <c r="B528" t="s">
+        <v>11</v>
+      </c>
+      <c r="C528" t="s">
+        <v>17</v>
+      </c>
+      <c r="D528" s="2">
+        <v>78600000</v>
+      </c>
+    </row>
+    <row r="529" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A529">
+        <v>2017</v>
+      </c>
+      <c r="B529" t="s">
+        <v>11</v>
+      </c>
+      <c r="C529" t="s">
+        <v>17</v>
+      </c>
+      <c r="D529" s="2">
+        <v>96200000</v>
+      </c>
+    </row>
+    <row r="530" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A530">
+        <v>2018</v>
+      </c>
+      <c r="B530" t="s">
+        <v>11</v>
+      </c>
+      <c r="C530" t="s">
+        <v>17</v>
+      </c>
+      <c r="D530" s="2">
+        <v>114400000</v>
+      </c>
+    </row>
+    <row r="531" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A531">
+        <v>2019</v>
+      </c>
+      <c r="B531" t="s">
+        <v>11</v>
+      </c>
+      <c r="C531" t="s">
+        <v>17</v>
+      </c>
+      <c r="D531" s="2">
+        <v>95400000</v>
+      </c>
+    </row>
+    <row r="532" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A532">
+        <v>2020</v>
+      </c>
+      <c r="B532" t="s">
+        <v>11</v>
+      </c>
+      <c r="C532" t="s">
+        <v>17</v>
+      </c>
+      <c r="D532" s="2">
+        <v>88300000</v>
+      </c>
+    </row>
+    <row r="533" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A533">
+        <v>2021</v>
+      </c>
+      <c r="B533" t="s">
+        <v>11</v>
+      </c>
+      <c r="C533" t="s">
+        <v>17</v>
+      </c>
+      <c r="D533" s="2">
+        <v>35800000</v>
+      </c>
+    </row>
+    <row r="534" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A534">
+        <v>2022</v>
+      </c>
+      <c r="B534" t="s">
+        <v>11</v>
+      </c>
+      <c r="C534" t="s">
+        <v>17</v>
+      </c>
+      <c r="D534" s="2">
+        <v>32600000</v>
+      </c>
+    </row>
+    <row r="535" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A535">
+        <v>2008</v>
+      </c>
+      <c r="B535" t="s">
+        <v>12</v>
+      </c>
+      <c r="C535" t="s">
+        <v>17</v>
+      </c>
+      <c r="D535" s="2">
+        <v>463800000</v>
+      </c>
+    </row>
+    <row r="536" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A536">
+        <v>2009</v>
+      </c>
+      <c r="B536" t="s">
+        <v>12</v>
+      </c>
+      <c r="C536" t="s">
+        <v>17</v>
+      </c>
+      <c r="D536" s="2">
+        <v>397400000</v>
+      </c>
+    </row>
+    <row r="537" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A537">
+        <v>2010</v>
+      </c>
+      <c r="B537" t="s">
+        <v>12</v>
+      </c>
+      <c r="C537" t="s">
+        <v>17</v>
+      </c>
+      <c r="D537" s="2">
+        <v>400900000</v>
+      </c>
+    </row>
+    <row r="538" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A538">
+        <v>2011</v>
+      </c>
+      <c r="B538" t="s">
+        <v>12</v>
+      </c>
+      <c r="C538" t="s">
+        <v>17</v>
+      </c>
+      <c r="D538" s="2">
+        <v>416500000</v>
+      </c>
+    </row>
+    <row r="539" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A539">
+        <v>2012</v>
+      </c>
+      <c r="B539" t="s">
+        <v>12</v>
+      </c>
+      <c r="C539" t="s">
+        <v>17</v>
+      </c>
+      <c r="D539" s="2">
+        <v>400400000</v>
+      </c>
+    </row>
+    <row r="540" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A540">
+        <v>2013</v>
+      </c>
+      <c r="B540" t="s">
+        <v>12</v>
+      </c>
+      <c r="C540" t="s">
+        <v>17</v>
+      </c>
+      <c r="D540" s="2">
+        <v>414700000</v>
+      </c>
+    </row>
+    <row r="541" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A541">
+        <v>2014</v>
+      </c>
+      <c r="B541" t="s">
+        <v>12</v>
+      </c>
+      <c r="C541" t="s">
+        <v>17</v>
+      </c>
+      <c r="D541" s="2">
+        <v>404700000</v>
+      </c>
+    </row>
+    <row r="542" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A542">
+        <v>2015</v>
+      </c>
+      <c r="B542" t="s">
+        <v>12</v>
+      </c>
+      <c r="C542" t="s">
+        <v>17</v>
+      </c>
+      <c r="D542" s="2">
+        <v>418900000</v>
+      </c>
+    </row>
+    <row r="543" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A543">
+        <v>2016</v>
+      </c>
+      <c r="B543" t="s">
+        <v>12</v>
+      </c>
+      <c r="C543" t="s">
+        <v>17</v>
+      </c>
+      <c r="D543" s="2">
+        <v>379000000</v>
+      </c>
+    </row>
+    <row r="544" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A544">
+        <v>2017</v>
+      </c>
+      <c r="B544" t="s">
+        <v>12</v>
+      </c>
+      <c r="C544" t="s">
+        <v>17</v>
+      </c>
+      <c r="D544" s="2">
+        <v>345400000</v>
+      </c>
+    </row>
+    <row r="545" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A545">
+        <v>2018</v>
+      </c>
+      <c r="B545" t="s">
+        <v>12</v>
+      </c>
+      <c r="C545" t="s">
+        <v>17</v>
+      </c>
+      <c r="D545" s="2">
+        <v>348700000</v>
+      </c>
+    </row>
+    <row r="546" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A546">
+        <v>2019</v>
+      </c>
+      <c r="B546" t="s">
+        <v>12</v>
+      </c>
+      <c r="C546" t="s">
+        <v>17</v>
+      </c>
+      <c r="D546" s="2">
+        <v>357300000</v>
+      </c>
+    </row>
+    <row r="547" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A547">
+        <v>2020</v>
+      </c>
+      <c r="B547" t="s">
+        <v>12</v>
+      </c>
+      <c r="C547" t="s">
+        <v>17</v>
+      </c>
+      <c r="D547" s="2">
+        <v>360400000</v>
+      </c>
+    </row>
+    <row r="548" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A548">
+        <v>2021</v>
+      </c>
+      <c r="B548" t="s">
+        <v>12</v>
+      </c>
+      <c r="C548" t="s">
+        <v>17</v>
+      </c>
+      <c r="D548" s="2">
+        <v>326600000</v>
+      </c>
+    </row>
+    <row r="549" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A549">
+        <v>2022</v>
+      </c>
+      <c r="B549" t="s">
+        <v>12</v>
+      </c>
+      <c r="C549" t="s">
+        <v>17</v>
+      </c>
+      <c r="D549" s="2">
+        <v>278500000</v>
+      </c>
+    </row>
+    <row r="550" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A550">
+        <v>2008</v>
+      </c>
+      <c r="B550" t="s">
+        <v>10</v>
+      </c>
+      <c r="C550" t="s">
+        <v>17</v>
+      </c>
+      <c r="D550" s="2">
+        <v>13400000</v>
+      </c>
+    </row>
+    <row r="551" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A551">
+        <v>2009</v>
+      </c>
+      <c r="B551" t="s">
+        <v>10</v>
+      </c>
+      <c r="C551" t="s">
+        <v>17</v>
+      </c>
+      <c r="D551" s="2">
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="552" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A552">
+        <v>2010</v>
+      </c>
+      <c r="B552" t="s">
+        <v>10</v>
+      </c>
+      <c r="C552" t="s">
+        <v>17</v>
+      </c>
+      <c r="D552" s="2">
+        <v>2600000</v>
+      </c>
+    </row>
+    <row r="553" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A553">
+        <v>2011</v>
+      </c>
+      <c r="B553" t="s">
+        <v>10</v>
+      </c>
+      <c r="C553" t="s">
+        <v>17</v>
+      </c>
+      <c r="D553" s="2">
+        <v>2400000</v>
+      </c>
+    </row>
+    <row r="554" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A554">
+        <v>2012</v>
+      </c>
+      <c r="B554" t="s">
+        <v>10</v>
+      </c>
+      <c r="C554" t="s">
+        <v>17</v>
+      </c>
+      <c r="D554" s="2">
+        <v>19700000</v>
+      </c>
+    </row>
+    <row r="555" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A555">
+        <v>2013</v>
+      </c>
+      <c r="B555" t="s">
+        <v>10</v>
+      </c>
+      <c r="C555" t="s">
+        <v>17</v>
+      </c>
+      <c r="D555" s="2">
+        <v>15200000</v>
+      </c>
+    </row>
+    <row r="556" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A556">
+        <v>2014</v>
+      </c>
+      <c r="B556" t="s">
+        <v>10</v>
+      </c>
+      <c r="C556" t="s">
+        <v>17</v>
+      </c>
+      <c r="D556" s="2">
+        <v>4300000</v>
+      </c>
+    </row>
+    <row r="557" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A557">
+        <v>2015</v>
+      </c>
+      <c r="B557" t="s">
+        <v>10</v>
+      </c>
+      <c r="C557" t="s">
+        <v>17</v>
+      </c>
+      <c r="D557" s="2">
+        <v>2300000</v>
+      </c>
+    </row>
+    <row r="558" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A558">
+        <v>2016</v>
+      </c>
+      <c r="B558" t="s">
+        <v>10</v>
+      </c>
+      <c r="C558" t="s">
+        <v>17</v>
+      </c>
+      <c r="D558" s="2">
+        <v>3400000</v>
+      </c>
+    </row>
+    <row r="559" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A559">
+        <v>2017</v>
+      </c>
+      <c r="B559" t="s">
+        <v>10</v>
+      </c>
+      <c r="C559" t="s">
+        <v>17</v>
+      </c>
+      <c r="D559" s="2">
+        <v>5800000</v>
+      </c>
+    </row>
+    <row r="560" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A560">
+        <v>2018</v>
+      </c>
+      <c r="B560" t="s">
+        <v>10</v>
+      </c>
+      <c r="C560" t="s">
+        <v>17</v>
+      </c>
+      <c r="D560" s="2">
+        <v>18500000</v>
+      </c>
+    </row>
+    <row r="561" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A561">
+        <v>2019</v>
+      </c>
+      <c r="B561" t="s">
+        <v>10</v>
+      </c>
+      <c r="C561" t="s">
+        <v>17</v>
+      </c>
+      <c r="D561" s="2">
+        <v>5800000</v>
+      </c>
+    </row>
+    <row r="562" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A562">
+        <v>2020</v>
+      </c>
+      <c r="B562" t="s">
+        <v>10</v>
+      </c>
+      <c r="C562" t="s">
+        <v>17</v>
+      </c>
+      <c r="D562" s="2">
+        <v>6900000</v>
+      </c>
+    </row>
+    <row r="563" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A563">
+        <v>2021</v>
+      </c>
+      <c r="B563" t="s">
+        <v>10</v>
+      </c>
+      <c r="C563" t="s">
+        <v>17</v>
+      </c>
+      <c r="D563" s="2">
+        <v>5300000</v>
+      </c>
+    </row>
+    <row r="564" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A564">
+        <v>2022</v>
+      </c>
+      <c r="B564" t="s">
+        <v>10</v>
+      </c>
+      <c r="C564" t="s">
+        <v>17</v>
+      </c>
+      <c r="D564" s="2">
+        <v>5300000</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D429" xr:uid="{47F90730-DE6E-4990-B5C3-FD64641F0A26}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>